<commit_message>
troca da biblioteca pandas pela openpyxl
</commit_message>
<xml_diff>
--- a/contas.xlsx
+++ b/contas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LOURENXX\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LOURENXX\Desktop\automacao_instragram\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,13 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="contas">Plan1!$A$1</definedName>
+    <definedName name="contas_instagram">Plan1!$A$1</definedName>
+    <definedName name="Contatos">Plan1!$A$1</definedName>
+    <definedName name="insta_contas">Plan1!$A$1</definedName>
+    <definedName name="perfil">Plan1!$A:$A</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -346,7 +353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
atualização de todos os xpaths e criação de um novo loop for com o openpyxl
</commit_message>
<xml_diff>
--- a/contas.xlsx
+++ b/contas.xlsx
@@ -33,7 +33,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>lourenxx_g</t>
+    <t>julianabap.13</t>
   </si>
 </sst>
 </file>
@@ -353,9 +353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
limpando a planinha 'contas'
</commit_message>
<xml_diff>
--- a/contas.xlsx
+++ b/contas.xlsx
@@ -31,11 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>julianabap.13</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,13 +352,7 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alterando xpath linha 74
</commit_message>
<xml_diff>
--- a/contas.xlsx
+++ b/contas.xlsx
@@ -31,7 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>lourenxx_g</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,7 +356,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alterações para o funcionamento do programa
</commit_message>
<xml_diff>
--- a/contas.xlsx
+++ b/contas.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="contas">Plan1!$A$1</definedName>
-    <definedName name="contas_instagram">Plan1!$A$1</definedName>
-    <definedName name="Contatos">Plan1!$A$1</definedName>
-    <definedName name="insta_contas">Plan1!$A$1</definedName>
+    <definedName name="contas">Plan1!#REF!</definedName>
+    <definedName name="contas_instagram">Plan1!#REF!</definedName>
+    <definedName name="Contatos">Plan1!#REF!</definedName>
+    <definedName name="insta_contas">Plan1!#REF!</definedName>
     <definedName name="perfil">Plan1!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,11 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>julianabap.13</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -353,16 +349,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>